<commit_message>
import excel todo: upload excel mau
</commit_message>
<xml_diff>
--- a/public/download/Candidate.xlsx
+++ b/public/download/Candidate.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinh Nguyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF095EDA-556E-4583-80EB-D998F639B384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBE3CC6-54AC-4B11-B1DD-8AE5AA660BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Candidate" sheetId="1" r:id="rId1"/>
+    <sheet name="B1" sheetId="1" r:id="rId1"/>
+    <sheet name="B2" sheetId="2" r:id="rId2"/>
+    <sheet name="C" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -42,12 +44,6 @@
     <t>Số điện thoại</t>
   </si>
   <si>
-    <t>Loại khóa học</t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
     <t>Ngày sinh</t>
   </si>
   <si>
@@ -78,9 +74,6 @@
     <t xml:space="preserve"> Nơi cấp giấy phép lái xe 2 bánh</t>
   </si>
   <si>
-    <t xml:space="preserve">Có giấy khám sức khoẻ chưa ? </t>
-  </si>
-  <si>
     <t>Ngày khám sức khoẻ</t>
   </si>
   <si>
@@ -96,19 +89,22 @@
     <t>0348200824</t>
   </si>
   <si>
-    <t>B2</t>
+    <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>Sài Gòn</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
-    <t>Sài Gòn</t>
-  </si>
-  <si>
-    <t>Chưa</t>
+    <t>Giới tính(nam hoặc nữ)</t>
+  </si>
+  <si>
+    <t>Có giấy khám sức khoẻ chưa ? (có hoặc chưa)</t>
+  </si>
+  <si>
+    <t>Có</t>
   </si>
 </sst>
 </file>
@@ -119,7 +115,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,6 +136,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -501,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,14 +516,16 @@
     <col min="3" max="3" width="10.54296875" customWidth="1"/>
     <col min="4" max="4" width="25.54296875" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" customWidth="1"/>
-    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="65" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,227 +542,384 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4">
+        <v>36336</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4">
+        <v>36336</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="M4" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4DCC58-C56F-4D71-B5AC-9B43084684E4}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:18" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4">
+        <v>36336</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252BAAA8-1B5C-4273-9EBC-59DF71AD86DD}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:18" ht="65.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4">
+        <v>36336</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="4">
-        <v>36336</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4">
-        <v>36336</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="4">
-        <v>36336</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>